<commit_message>
Adds functionality of moving processed file to Processed. Bug fixes for handling number and date values in excel.
</commit_message>
<xml_diff>
--- a/DataFiles/study02/test01.xlsx
+++ b/DataFiles/study02/test01.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\MoTrPac_API\ProgrammaticConnectivity\MountSinai_metadata_file_loader\study02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\MoTrPac_API\ProgrammaticConnectivity\MountSinai_metadata_file_loader\DataFiles\study02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC34D2B-AC1A-42AD-AD8C-248CB5AEC723}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0103D87B-D754-4B11-B7D3-8B55DADF572C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11265" xr2:uid="{8B41012A-54BD-465D-9D80-AA2D8EC80760}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{8B41012A-54BD-465D-9D80-AA2D8EC80760}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Page2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Exc_Col1</t>
   </si>
@@ -90,6 +91,18 @@
   </si>
   <si>
     <t>Col4_Row4</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
@@ -131,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1645BE06-C88E-498D-8A50-64C7FD02F547}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,4 +546,90 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA3467B-4D45-40BF-B186-ACA9D529E3A0}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43497</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43498</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43499</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43500</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds logging functionality. Work in progress.
</commit_message>
<xml_diff>
--- a/DataFiles/study02/test01.xlsx
+++ b/DataFiles/study02/test01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\MoTrPac_API\ProgrammaticConnectivity\MountSinai_metadata_file_loader\DataFiles\study02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0103D87B-D754-4B11-B7D3-8B55DADF572C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1814764C-90CA-40EA-89B7-653D4DC81D04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{8B41012A-54BD-465D-9D80-AA2D8EC80760}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8B41012A-54BD-465D-9D80-AA2D8EC80760}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>

</xml_diff>